<commit_message>
Add a nested dictionary for storing Exceptions (to output in SAM)
</commit_message>
<xml_diff>
--- a/landbosse/landbosse_api/project_list.xlsx
+++ b/landbosse/landbosse_api/project_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/landbosse/landbosse_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D4BA6D-4D56-B348-9612-66066C1C2190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C3A26F-4F4D-204F-A600-3588AB7252A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="78260" yWindow="2300" windowWidth="12800" windowHeight="16500" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Project list" sheetId="1" r:id="rId1"/>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update exception handling for SAM
</commit_message>
<xml_diff>
--- a/landbosse/landbosse_api/project_list.xlsx
+++ b/landbosse/landbosse_api/project_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/landbosse/landbosse_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C3A26F-4F4D-204F-A600-3588AB7252A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA25FBB-47BD-EA46-9E85-FE0EA60B95D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Project list" sheetId="1" r:id="rId1"/>
     <sheet name="Parametric list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -203,12 +203,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +527,7 @@
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -700,7 +701,7 @@
       <c r="C2">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>1.5</v>
       </c>
       <c r="E2">

</xml_diff>

<commit_message>
Modify default user inputs spreadsheet, And replace 99s in project data spreadsheet with publicly available data
</commit_message>
<xml_diff>
--- a/landbosse/landbosse_api/project_list.xlsx
+++ b/landbosse/landbosse_api/project_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/landbosse/landbosse_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA25FBB-47BD-EA46-9E85-FE0EA60B95D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D87E72C-0012-7446-91EE-316AA149D256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="3140" yWindow="4720" windowWidth="28800" windowHeight="7520" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Project list" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Project ID</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Crane breakdown fraction</t>
+  </si>
+  <si>
+    <t>project_data_defaults</t>
   </si>
 </sst>
 </file>
@@ -527,7 +530,7 @@
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,7 +699,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -717,7 +720,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="J2">
         <v>0.7</v>
@@ -759,10 +762,10 @@
         <v>15</v>
       </c>
       <c r="W2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="X2">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="Y2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Manual mode and Auto mode are functional and show functional differences.
</commit_message>
<xml_diff>
--- a/landbosse/landbosse_api/project_list.xlsx
+++ b/landbosse/landbosse_api/project_list.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbhaskar/Desktop/Projects/public_landbosse/LandBOSSE/landbosse/landbosse_api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ccampos/PycharmProjects/LandBOSSE/input/project_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A522B529-4B70-2F44-9A51-53DE3462AAAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E61BEE7-40D1-2C4B-9569-93A5932F6C51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14360" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
+    <workbookView xWindow="840" yWindow="4260" windowWidth="16900" windowHeight="10920" xr2:uid="{CA848B2B-50AD-1141-9E6B-5049DCE507C8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Project list" sheetId="1" r:id="rId1"/>
+    <sheet name="Parametric list" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Project ID</t>
   </si>
@@ -98,91 +99,91 @@
     <t>Non-Erection Wind Delay Critical Speed (m/s)</t>
   </si>
   <si>
+    <t>Interconnect Voltage (kV)</t>
+  </si>
+  <si>
+    <t>New Switchyard (y/n)</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Road length adder (m)</t>
+  </si>
+  <si>
+    <t>Road Quality (0-1)</t>
+  </si>
+  <si>
+    <t>Percent of roads that will be constructed</t>
+  </si>
+  <si>
+    <t>Road width (ft)</t>
+  </si>
+  <si>
+    <t>Road thickness (in)</t>
+  </si>
+  <si>
+    <t>Crane width (m)</t>
+  </si>
+  <si>
+    <t>Number of highway permits</t>
+  </si>
+  <si>
+    <t>Number of access roads</t>
+  </si>
+  <si>
+    <t>Overtime multiplier</t>
+  </si>
+  <si>
+    <t>Allow same flag</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Markup contingency</t>
+  </si>
+  <si>
+    <t>Markup warranty management</t>
+  </si>
+  <si>
+    <t>Markup sales and use tax</t>
+  </si>
+  <si>
+    <t>Markup overhead</t>
+  </si>
+  <si>
+    <t>Markup profit margin</t>
+  </si>
+  <si>
+    <t>Project data file</t>
+  </si>
+  <si>
+    <t>Crane breakdown fraction</t>
+  </si>
+  <si>
+    <t>Labor cost multiplier</t>
+  </si>
+  <si>
+    <t>Override total management cost for distributed (0 does not override)</t>
+  </si>
+  <si>
+    <t>Calculate road cost for distributed wind? (y/n)</t>
+  </si>
+  <si>
+    <t>Site prep area for Distributed wind (m2)</t>
+  </si>
+  <si>
+    <t>project_data_defaults</t>
+  </si>
+  <si>
+    <t>Collection mode</t>
+  </si>
+  <si>
     <t>Distance to interconnect (miles)</t>
   </si>
   <si>
-    <t>Interconnect Voltage (kV)</t>
-  </si>
-  <si>
-    <t>New Switchyard (y/n)</t>
-  </si>
-  <si>
-    <t>Road length adder (m)</t>
-  </si>
-  <si>
-    <t>Road Quality (0-1)</t>
-  </si>
-  <si>
-    <t>Percent of roads that will be constructed</t>
-  </si>
-  <si>
-    <t>Road width (ft)</t>
-  </si>
-  <si>
-    <t>Road thickness (in)</t>
-  </si>
-  <si>
-    <t>Crane width (m)</t>
-  </si>
-  <si>
-    <t>Number of highway permits</t>
-  </si>
-  <si>
-    <t>Number of access roads</t>
-  </si>
-  <si>
-    <t>Overtime multiplier</t>
-  </si>
-  <si>
-    <t>Allow same flag</t>
-  </si>
-  <si>
-    <t>Markup contingency</t>
-  </si>
-  <si>
-    <t>Markup warranty management</t>
-  </si>
-  <si>
-    <t>Markup sales and use tax</t>
-  </si>
-  <si>
-    <t>Markup overhead</t>
-  </si>
-  <si>
-    <t>Markup profit margin</t>
-  </si>
-  <si>
-    <t>Project data file</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Calculate road cost for distributed wind? (y/n)</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>Site prep area for Distributed wind (m2)</t>
-  </si>
-  <si>
-    <t>Override total management cost for distributed (0 does not override)</t>
-  </si>
-  <si>
-    <t>Utility Interconnection Fees (Small DW only)</t>
-  </si>
-  <si>
-    <t>Labor cost multiplier</t>
-  </si>
-  <si>
-    <t>Crane breakdown fraction</t>
-  </si>
-  <si>
-    <t>ge15_public</t>
-  </si>
-  <si>
-    <t>foundation_validation_ge15</t>
+    <t>auto</t>
   </si>
 </sst>
 </file>
@@ -208,14 +209,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,23 +241,26 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -568,208 +572,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978C2AE7-DAF9-A64F-82B2-BFC05FEB6151}">
-  <dimension ref="A1:AT5"/>
+  <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="28.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="1" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="18" style="1" customWidth="1"/>
-    <col min="18" max="18" width="27.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="52.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.5" style="1" customWidth="1"/>
-    <col min="22" max="22" width="39.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20" style="1" customWidth="1"/>
-    <col min="27" max="27" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="28.1640625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="25.5" style="1" customWidth="1"/>
-    <col min="31" max="31" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="39.6640625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="23" style="1" customWidth="1"/>
-    <col min="34" max="34" width="27.5" style="1" customWidth="1"/>
-    <col min="35" max="35" width="22.1640625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="24.6640625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="26.6640625" style="1" customWidth="1"/>
-    <col min="38" max="38" width="60.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="32" style="1" customWidth="1"/>
-    <col min="40" max="40" width="27.1640625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="22.6640625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="34" style="1" customWidth="1"/>
-    <col min="43" max="43" width="24.6640625" style="1" customWidth="1"/>
-    <col min="44" max="44" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="22.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="11.1640625" style="1"/>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
+    <col min="18" max="18" width="27.33203125" customWidth="1"/>
+    <col min="19" max="19" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="46" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.5" customWidth="1"/>
+    <col min="22" max="22" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20" customWidth="1"/>
+    <col min="27" max="27" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.33203125" customWidth="1"/>
+    <col min="30" max="30" width="25.5" customWidth="1"/>
+    <col min="31" max="31" width="23" customWidth="1"/>
+    <col min="32" max="32" width="27.5" customWidth="1"/>
+    <col min="33" max="33" width="22.33203125" customWidth="1"/>
+    <col min="34" max="34" width="24.83203125" customWidth="1"/>
+    <col min="35" max="35" width="26.6640625" customWidth="1"/>
+    <col min="36" max="36" width="32" customWidth="1"/>
+    <col min="37" max="37" width="27.33203125" customWidth="1"/>
+    <col min="38" max="38" width="22.6640625" customWidth="1"/>
+    <col min="39" max="39" width="34" customWidth="1"/>
+    <col min="40" max="40" width="24.83203125" customWidth="1"/>
+    <col min="41" max="41" width="24.5" customWidth="1"/>
+    <col min="42" max="42" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AO1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AP1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AG1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AR1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AM1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AS1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AS1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>48</v>
+      <c r="B2" t="s">
+        <v>46</v>
       </c>
       <c r="C2" s="1">
         <v>9</v>
@@ -790,7 +793,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1">
         <v>0.8</v>
@@ -807,7 +810,7 @@
       <c r="N2" s="1">
         <v>2.36</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>589000</v>
       </c>
       <c r="P2" s="1">
@@ -823,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="1">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="U2" s="1">
         <v>10</v>
@@ -831,91 +834,121 @@
       <c r="V2" s="1">
         <v>15</v>
       </c>
-      <c r="W2" s="2">
-        <v>5</v>
-      </c>
-      <c r="X2" s="2">
+      <c r="W2" s="4">
+        <v>10</v>
+      </c>
+      <c r="X2" s="4">
         <v>130</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" s="2">
+      <c r="Y2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="4">
         <v>5000</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="4">
         <v>0.6</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="5">
         <v>0.33</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="4">
         <v>20</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="4">
         <v>8</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF2" s="1">
+      <c r="AE2" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="AK2" s="4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AL2" s="4">
         <v>0</v>
       </c>
-      <c r="AG2" s="2">
-        <v>12.2</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>10</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL2" s="5">
+      <c r="AM2" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="AN2" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="AO2" s="4">
         <v>0</v>
       </c>
-      <c r="AM2" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="AO2" s="2">
+      <c r="AP2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="9">
         <v>0</v>
       </c>
-      <c r="AP2" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="AQ2" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="AR2" s="2">
+      <c r="AR2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AS2" s="7">
         <v>0</v>
       </c>
-      <c r="AS2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="2">
-        <v>0</v>
+      <c r="AT2" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A3"/>
+      <c r="A3" s="1"/>
+      <c r="O3" s="3"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="9"/>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="Z4" s="2"/>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="Z5" s="2"/>
+      <c r="O4" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E56176-3BBC-8645-BA4C-0420D94797E1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>